<commit_message>
aggiunta tor-causale-orig e verifica in assegnazione protocollo
</commit_message>
<xml_diff>
--- a/CAMBIO RIORDINO.xlsx
+++ b/CAMBIO RIORDINO.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Lubex\GESLUX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A9DC9E6-4FD1-4887-A26E-AB3A74A51476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6962B9-766A-47FD-94F4-C86794525F00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -758,7 +758,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
aggiunte qtqa riordino, testate su programmazione, da vedere in singola. Eliminare poi le forzature di crea-ordfor e pordini
</commit_message>
<xml_diff>
--- a/CAMBIO RIORDINO.xlsx
+++ b/CAMBIO RIORDINO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Lubex\GESLUX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6962B9-766A-47FD-94F4-C86794525F00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6A34B4-90E1-4A78-93D5-D54E0F137341}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>